<commit_message>
retro + excel update
</commit_message>
<xml_diff>
--- a/Abgaben/Group_A_TaskRisk_log.xlsx
+++ b/Abgaben/Group_A_TaskRisk_log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0D28CC-17B2-435F-9CDB-0A193E965776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1770E574-4F72-4DCA-B44A-527CA7B264EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="185">
   <si>
     <t>#</t>
   </si>
@@ -431,9 +431,6 @@
     <t>Testing communication with MongoDB</t>
   </si>
   <si>
-    <t xml:space="preserve">Create view </t>
-  </si>
-  <si>
     <t>Research for MVC-Pattern in NodeJs</t>
   </si>
   <si>
@@ -470,9 +467,6 @@
     <t>37.7</t>
   </si>
   <si>
-    <t>37.8</t>
-  </si>
-  <si>
     <t>Creating a plan for refactoring</t>
   </si>
   <si>
@@ -485,9 +479,6 @@
     <t>Download component</t>
   </si>
   <si>
-    <t>Creating a view</t>
-  </si>
-  <si>
     <t>Time component</t>
   </si>
   <si>
@@ -510,6 +501,93 @@
   </si>
   <si>
     <t>34.3</t>
+  </si>
+  <si>
+    <t>Implenting upload to database</t>
+  </si>
+  <si>
+    <t>Downloading from database</t>
+  </si>
+  <si>
+    <t>37.7.1</t>
+  </si>
+  <si>
+    <t>37.7.2.</t>
+  </si>
+  <si>
+    <t>Upload to database available</t>
+  </si>
+  <si>
+    <t>Download to database available</t>
+  </si>
+  <si>
+    <t>39.1</t>
+  </si>
+  <si>
+    <t>Upload function</t>
+  </si>
+  <si>
+    <t>Excel file can be uploaded temporaly into Server</t>
+  </si>
+  <si>
+    <t>39.2</t>
+  </si>
+  <si>
+    <t>Data cleaning</t>
+  </si>
+  <si>
+    <t>All rows in the table which contains empty cells should be ignored and not converted to Application Object</t>
+  </si>
+  <si>
+    <t>39.3</t>
+  </si>
+  <si>
+    <t>Add the imported apps to the diagram</t>
+  </si>
+  <si>
+    <t>Imported Application should be added and shown in the diagram</t>
+  </si>
+  <si>
+    <t>Research for making Data Object reusable</t>
+  </si>
+  <si>
+    <t>Evaluate in which ways we can implent this task</t>
+  </si>
+  <si>
+    <t>38.1</t>
+  </si>
+  <si>
+    <t>38.2</t>
+  </si>
+  <si>
+    <t>Implenting a function to read and save all Data Objects and its values</t>
+  </si>
+  <si>
+    <t>Making sure that we can work with the Data Objects and its values</t>
+  </si>
+  <si>
+    <t>Add this function into the listener and making sure it won't save duplicates</t>
+  </si>
+  <si>
+    <t>Function to read and save Data Objects by name</t>
+  </si>
+  <si>
+    <t>Implenting dropdown option for loading presets (Data Objects by name)</t>
+  </si>
+  <si>
+    <t>Implenting function into listener to fill Data Objects with the selected values from preset</t>
+  </si>
+  <si>
+    <t>38.3</t>
+  </si>
+  <si>
+    <t>38.4</t>
+  </si>
+  <si>
+    <t>38.5</t>
+  </si>
+  <si>
+    <t>38.6</t>
   </si>
 </sst>
 </file>
@@ -704,7 +782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -784,6 +862,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1174,8 +1256,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="A3:I51" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A3:I51" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="A3:I61" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+  <autoFilter ref="A3:I61" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task" dataDxfId="19"/>
@@ -1498,17 +1580,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="121" customWidth="1"/>
-    <col min="3" max="3" width="83.140625" customWidth="1"/>
+    <col min="3" max="3" width="91.140625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" style="22" customWidth="1"/>
@@ -2403,7 +2485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>30</v>
       </c>
@@ -2432,7 +2514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>31</v>
       </c>
@@ -2461,7 +2543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>32</v>
       </c>
@@ -2483,10 +2565,14 @@
       <c r="G35" s="14">
         <v>3</v>
       </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14"/>
-    </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H35" s="13">
+        <v>3</v>
+      </c>
+      <c r="I35" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>33</v>
       </c>
@@ -2515,15 +2601,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D37" s="13" t="s">
         <v>34</v>
@@ -2543,16 +2629,17 @@
       <c r="I37" s="14">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L37" s="32"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>34</v>
@@ -2572,16 +2659,17 @@
       <c r="I38" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L38" s="32"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D39" s="13" t="s">
         <v>34</v>
@@ -2601,8 +2689,9 @@
       <c r="I39" s="14">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L39" s="32"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="24">
         <v>35</v>
       </c>
@@ -2630,8 +2719,9 @@
       <c r="I40" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L40" s="32"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="24">
         <v>36</v>
       </c>
@@ -2639,7 +2729,7 @@
         <v>125</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D41" s="15"/>
       <c r="E41" s="15"/>
@@ -2647,16 +2737,17 @@
       <c r="G41" s="16"/>
       <c r="H41" s="15"/>
       <c r="I41" s="16"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L41" s="32"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B42" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" s="13" t="s">
         <v>133</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>134</v>
       </c>
       <c r="D42" s="13" t="s">
         <v>31</v>
@@ -2677,15 +2768,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D43" s="13" t="s">
         <v>31</v>
@@ -2706,22 +2797,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B44" s="27" t="s">
         <v>127</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D44" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E44" s="15" t="s">
-        <v>28</v>
-      </c>
       <c r="F44" s="20">
         <v>3</v>
       </c>
@@ -2735,15 +2826,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B45" s="27" t="s">
         <v>130</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>28</v>
@@ -2764,15 +2855,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B46" s="27" t="s">
         <v>129</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>31</v>
@@ -2786,133 +2877,411 @@
       <c r="G46" s="16">
         <v>3</v>
       </c>
-      <c r="H46" s="15"/>
-      <c r="I46" s="16"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
+      <c r="H46" s="15">
+        <v>3</v>
+      </c>
+      <c r="I46" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F47" s="20">
+        <v>3</v>
+      </c>
+      <c r="G47" s="16">
+        <v>3</v>
+      </c>
+      <c r="H47" s="15">
+        <v>3</v>
+      </c>
+      <c r="I47" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B47" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F47" s="20">
-        <v>3</v>
-      </c>
-      <c r="G47" s="14">
-        <v>3</v>
-      </c>
-      <c r="H47" s="13"/>
-      <c r="I47" s="14"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
-        <v>144</v>
-      </c>
       <c r="B48" s="27" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F48" s="20">
-        <v>3</v>
-      </c>
-      <c r="G48" s="16">
-        <v>3</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="16"/>
       <c r="H48" s="15"/>
       <c r="I48" s="16"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B49" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D49" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E49" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="F49" s="20">
+        <v>3</v>
+      </c>
+      <c r="G49" s="14">
+        <v>6</v>
+      </c>
+      <c r="H49" s="13">
+        <v>3</v>
+      </c>
+      <c r="I49" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B50" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F49" s="20">
-        <v>3</v>
-      </c>
-      <c r="G49" s="16">
+      <c r="F50" s="20">
+        <v>3</v>
+      </c>
+      <c r="G50" s="14">
+        <v>2</v>
+      </c>
+      <c r="H50" s="13">
+        <v>3</v>
+      </c>
+      <c r="I50" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="11">
+        <v>38</v>
+      </c>
+      <c r="B51" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="16"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="20">
+        <v>3</v>
+      </c>
+      <c r="G52" s="14">
+        <v>3</v>
+      </c>
+      <c r="H52" s="13">
+        <v>3</v>
+      </c>
+      <c r="I52" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F53" s="20">
+        <v>3</v>
+      </c>
+      <c r="G53" s="14">
+        <v>3</v>
+      </c>
+      <c r="H53" s="13">
+        <v>3</v>
+      </c>
+      <c r="I53" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54" s="20">
+        <v>3</v>
+      </c>
+      <c r="G54" s="14">
+        <v>2</v>
+      </c>
+      <c r="H54" s="13">
+        <v>3</v>
+      </c>
+      <c r="I54" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F55" s="20">
+        <v>3</v>
+      </c>
+      <c r="G55" s="14">
+        <v>3</v>
+      </c>
+      <c r="H55" s="13">
+        <v>3</v>
+      </c>
+      <c r="I55" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F56" s="20">
+        <v>3</v>
+      </c>
+      <c r="G56" s="14">
+        <v>2</v>
+      </c>
+      <c r="H56" s="13">
+        <v>3</v>
+      </c>
+      <c r="I56" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" s="20">
+        <v>3</v>
+      </c>
+      <c r="G57" s="14">
+        <v>3</v>
+      </c>
+      <c r="H57" s="13">
+        <v>3</v>
+      </c>
+      <c r="I57" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="24">
+        <v>39</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="14"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="B59" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F59" s="25">
+        <v>3</v>
+      </c>
+      <c r="G59" s="16">
+        <v>4</v>
+      </c>
+      <c r="H59" s="15">
+        <v>3</v>
+      </c>
+      <c r="I59" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="B60" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F60" s="25">
+        <v>3</v>
+      </c>
+      <c r="G60" s="16">
         <v>5</v>
       </c>
-      <c r="H49" s="15"/>
-      <c r="I49" s="16"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
-        <v>38</v>
-      </c>
-      <c r="B50" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="D50" s="15" t="s">
+      <c r="H60" s="15">
+        <v>3</v>
+      </c>
+      <c r="I60" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="B61" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="C61" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E50" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F50" s="25">
-        <v>3</v>
-      </c>
-      <c r="G50" s="16">
-        <v>6</v>
-      </c>
-      <c r="H50" s="15"/>
-      <c r="I50" s="16"/>
-    </row>
-    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="24">
-        <v>39</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F51" s="13">
-        <v>3</v>
-      </c>
-      <c r="G51" s="14">
-        <v>6</v>
-      </c>
-      <c r="H51" s="13"/>
-      <c r="I51" s="14"/>
+      <c r="F61" s="25">
+        <v>3</v>
+      </c>
+      <c r="G61" s="16">
+        <v>2</v>
+      </c>
+      <c r="H61" s="15">
+        <v>3</v>
+      </c>
+      <c r="I61" s="16">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Zeit für jeden in Tabelle
</commit_message>
<xml_diff>
--- a/Abgaben/Group_A_TaskRisk_log.xlsx
+++ b/Abgaben/Group_A_TaskRisk_log.xlsx
@@ -3,16 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1770E574-4F72-4DCA-B44A-527CA7B264EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120537C3-AEE0-470F-AFE9-0D364694BE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="13230" windowWidth="29040" windowHeight="15840" tabRatio="412" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Risks" sheetId="2" r:id="rId2"/>
-    <sheet name="Param" sheetId="6" state="hidden" r:id="rId3"/>
+    <sheet name="Time Spent" sheetId="7" r:id="rId3"/>
+    <sheet name="Param" sheetId="6" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="5" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="190">
   <si>
     <t>#</t>
   </si>
@@ -588,6 +592,21 @@
   </si>
   <si>
     <t>38.6</t>
+  </si>
+  <si>
+    <t>Spaltenbeschriftungen</t>
+  </si>
+  <si>
+    <t>(Leer)</t>
+  </si>
+  <si>
+    <t>Gesamtergebnis</t>
+  </si>
+  <si>
+    <t>Zeilenbeschriftungen</t>
+  </si>
+  <si>
+    <t>Summe von Real Effort in h</t>
   </si>
 </sst>
 </file>
@@ -782,7 +801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -859,13 +878,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1253,6 +1276,841 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Autor" refreshedDate="44361.453187962965" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="58" xr:uid="{098F87A3-12ED-4463-A2D5-46F8DF234481}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Tabelle2"/>
+  </cacheSource>
+  <cacheFields count="9">
+    <cacheField name="#" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="39"/>
+    </cacheField>
+    <cacheField name="Task" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Result" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Responsible" numFmtId="0">
+      <sharedItems containsBlank="1" count="7">
+        <s v="Karsten Rudolf"/>
+        <s v="Edgar Meilinger"/>
+        <s v="Ersan Ünsal"/>
+        <s v="Jan Leonardi"/>
+        <s v="Amine Amzil"/>
+        <s v="Gökhan Ünsal"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Support by" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Planned for Sprint #" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="3" count="5">
+        <n v="0"/>
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Planned Effort in h" numFmtId="164">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="6"/>
+    </cacheField>
+    <cacheField name="Realized in Sprint #" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="3" count="4">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Real Effort in h" numFmtId="164">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="6" count="10">
+        <s v="5min"/>
+        <s v="2min"/>
+        <n v="1"/>
+        <n v="0.5"/>
+        <n v="6"/>
+        <n v="3"/>
+        <n v="2"/>
+        <n v="5"/>
+        <n v="4"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="58">
+  <r>
+    <n v="1"/>
+    <s v="Creating a Discord Server for the Group"/>
+    <s v="Voice communication &amp; Filesharing"/>
+    <x v="0"/>
+    <s v="Team"/>
+    <x v="0"/>
+    <s v="5min"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="Creating a WhatsApp Group"/>
+    <s v="Text communication &amp; organising meetings"/>
+    <x v="1"/>
+    <s v="Team"/>
+    <x v="0"/>
+    <s v="2min"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <s v="Getting all phone numbers from teammembers for inviting them"/>
+    <s v="Having phone numbers for the WhatsApp Group"/>
+    <x v="2"/>
+    <s v="Team"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <s v="Setting up a first meeting in Discord"/>
+    <s v="Get to know each other"/>
+    <x v="3"/>
+    <s v="Team"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <s v="What development enviroment do we use ?"/>
+    <s v="all have the same development enviroment"/>
+    <x v="4"/>
+    <s v="Team"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <s v="First meeting: What VCS do we use ? "/>
+    <s v="sharing code &amp; version controlling"/>
+    <x v="2"/>
+    <s v="Team"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <s v="Setting up the VCS (GitHub)"/>
+    <s v="sharing code &amp; version controlling"/>
+    <x v="2"/>
+    <s v="Team"/>
+    <x v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <s v="getting started with node.js, express, GoJS"/>
+    <s v="understanding node.js, express, GoJS"/>
+    <x v="0"/>
+    <s v="Team"/>
+    <x v="0"/>
+    <n v="6"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <s v="Building a MindMap for the project"/>
+    <s v="Getting an overview for what we have so far (will be extended in the future)"/>
+    <x v="5"/>
+    <s v="Team"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <s v="Display Application - Canvas"/>
+    <s v="Visual Background Canvas"/>
+    <x v="3"/>
+    <s v="Karsten Rudolf, Edgar Meilinger"/>
+    <x v="1"/>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <s v="Display Application - Symbols"/>
+    <s v="Symbols can be created in the application"/>
+    <x v="3"/>
+    <s v="Karsten Rudolf, Edgar Meilinger"/>
+    <x v="1"/>
+    <n v="3"/>
+    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <s v="Display Application - Movement"/>
+    <s v="Elements can be moved freely in the application"/>
+    <x v="3"/>
+    <s v="Karsten Rudolf, Ersan Ünsal"/>
+    <x v="1"/>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <s v="Display Application - Symbol Palette"/>
+    <s v="Symbols can be dragged and dropped from the palette to the Main "/>
+    <x v="2"/>
+    <s v="Edgar Meilinger, Jan Leonardi"/>
+    <x v="1"/>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <s v="Display Application - CSS Design"/>
+    <s v="Application Design"/>
+    <x v="0"/>
+    <s v="Jan Leonardi, Ersan Ünsal"/>
+    <x v="1"/>
+    <n v="6"/>
+    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <s v="Application properties - Application documentation"/>
+    <s v="Basic documentation linked page for the customer"/>
+    <x v="2"/>
+    <s v="Edgar Meilinger"/>
+    <x v="1"/>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <s v="Application properties - properties window (name, version, description, COTS, release date, shutdown date)"/>
+    <s v="The properties can be shown using a properties window"/>
+    <x v="1"/>
+    <s v="Jan Leonardi, Gökhan Ünsal"/>
+    <x v="1"/>
+    <n v="4"/>
+    <x v="0"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <s v="Dataflows - Application linking"/>
+    <s v="Applications can be connected with directed associations (arrowheads) representing dataflows. "/>
+    <x v="4"/>
+    <s v="Gökhan Ünsal, Ersan Ünsal"/>
+    <x v="1"/>
+    <n v="6"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <s v="Data objects"/>
+    <s v="With following properties: Name, description &amp; personal data ? Dataflow refers to Data Object"/>
+    <x v="4"/>
+    <s v="Edgar Meilinger"/>
+    <x v="2"/>
+    <n v="4"/>
+    <x v="1"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <s v="Data objects design"/>
+    <s v="Label is like a node; display name, description &amp; personal data"/>
+    <x v="4"/>
+    <s v="Gökhan Ünsal"/>
+    <x v="2"/>
+    <n v="6"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <s v="Rename program to application"/>
+    <s v="Application will appear as default by the name &quot;Application&quot; and not as &quot;Program&quot;"/>
+    <x v="0"/>
+    <s v="Edgar Meilinger"/>
+    <x v="2"/>
+    <n v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="21"/>
+    <s v="Properties dialog windows is only visiable when clicked on (non selection = no properties window)"/>
+    <s v="Properties dialog will only be visible when you click on the Application"/>
+    <x v="3"/>
+    <s v="Karsten Rudolf"/>
+    <x v="2"/>
+    <n v="2"/>
+    <x v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <s v="Link property windows shows only &quot;name&quot; and &quot;color&quot; in property window"/>
+    <s v="Property window for links will only show &quot;name&quot; &amp; &quot;color&quot;"/>
+    <x v="4"/>
+    <s v="Jan Leonardi"/>
+    <x v="2"/>
+    <n v="2"/>
+    <x v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <s v="Research for: traffic light signals"/>
+    <s v="Gathering information about how GoJS saves data to use it for the traffic light"/>
+    <x v="0"/>
+    <s v="Ersan Ünsal"/>
+    <x v="2"/>
+    <n v="3"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <s v="Application: traffic light signals for release / shutdown date                _x000a_(blue = default, red = past shutdown date, amber = release date in future, green = in time between release &amp; shutdown date)"/>
+    <s v="Implementing traffic light system for Applications the have a visual overview for the status"/>
+    <x v="2"/>
+    <s v="Karsten Rudolf"/>
+    <x v="2"/>
+    <n v="5"/>
+    <x v="1"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <s v="3 dropdowns values for Cots: cots, propietary, undefined"/>
+    <s v="Changing free text value for COTS into a dropdown menu with 3 values(cots, propietary, undefined)"/>
+    <x v="0"/>
+    <s v="Ersan Ünsal"/>
+    <x v="2"/>
+    <n v="3"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <s v="Research for: Fields of decription a bit longer, several lines visible"/>
+    <s v="Change input filed to textarea"/>
+    <x v="1"/>
+    <s v="Jan Leonardi"/>
+    <x v="2"/>
+    <n v="3"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <s v="Graphical symbol for applications: applications need to be shown by a rectangle with two additional lines (as in the initial slide deck)."/>
+    <s v="Changing the visual desgin of the symbol for the applications"/>
+    <x v="1"/>
+    <s v="Ersan Ünsal"/>
+    <x v="2"/>
+    <n v="4"/>
+    <x v="1"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <s v="Research: How to export files with GoJS"/>
+    <s v="Being able to solve the export tasks"/>
+    <x v="3"/>
+    <s v="Amine Amzil"/>
+    <x v="2"/>
+    <n v="6"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <s v="Error Research: Output diagram object"/>
+    <s v="Diagramm data can be shown as JSON"/>
+    <x v="2"/>
+    <s v="Jan Leonardi"/>
+    <x v="2"/>
+    <n v="3"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="30"/>
+    <s v="Report data objects: A report is required so that all data objects in the application landscape can be exported as an file (csv)."/>
+    <s v="Implenting an export option to save &amp; report all data objects in the application landscape as an .csv file"/>
+    <x v="3"/>
+    <s v="Amine Amzil"/>
+    <x v="2"/>
+    <n v="4"/>
+    <x v="1"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <n v="31"/>
+    <s v="Setting up database and connection to the app"/>
+    <s v="Communication between app and database"/>
+    <x v="2"/>
+    <s v="Karsten Rudolf"/>
+    <x v="2"/>
+    <n v="3"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <s v="Fields of decription a bit longer, several lines visible"/>
+    <s v="Implementing more visible lines in the fields of description"/>
+    <x v="1"/>
+    <s v="Jan Leonardi"/>
+    <x v="2"/>
+    <n v="3"/>
+    <x v="2"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="33"/>
+    <s v="Report applications working with personal data: A report needs to be created that lists any application that works with personal data."/>
+    <s v="Implenting an export option to save &amp; report all data in the application related with personal data"/>
+    <x v="0"/>
+    <s v="Jan Leonardi"/>
+    <x v="3"/>
+    <n v="3"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="34.1"/>
+    <s v="Debugging"/>
+    <s v="Fixing bugs"/>
+    <x v="3"/>
+    <s v="Karsten Rudolf"/>
+    <x v="3"/>
+    <n v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="34.2"/>
+    <s v="Download component"/>
+    <s v="Download component"/>
+    <x v="3"/>
+    <s v="Karsten Rudolf"/>
+    <x v="3"/>
+    <n v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="34.3"/>
+    <s v="Time component"/>
+    <s v="Time component"/>
+    <x v="3"/>
+    <s v="Karsten Rudolf"/>
+    <x v="3"/>
+    <n v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="35"/>
+    <s v="Rename the Status to COTS Label"/>
+    <s v="Changing visual text from status to COTS"/>
+    <x v="2"/>
+    <s v="Edgar Meilinger"/>
+    <x v="3"/>
+    <n v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="36"/>
+    <s v="Refactoring the Code"/>
+    <s v="Application landscape has to be stored persistently e.g. as Database"/>
+    <x v="6"/>
+    <m/>
+    <x v="4"/>
+    <m/>
+    <x v="3"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="37.1"/>
+    <s v="Research for MVC-Pattern in NodeJs"/>
+    <s v="Using a Module for MVC Pattern"/>
+    <x v="2"/>
+    <s v="Amine Amzil"/>
+    <x v="3"/>
+    <n v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="37.2"/>
+    <s v="Creating a plan for refactoring"/>
+    <s v="Organising for the tasks to refactor the code"/>
+    <x v="2"/>
+    <s v="Amine Amzil"/>
+    <x v="3"/>
+    <n v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="37.3"/>
+    <s v="Generating a MVC Skeleton"/>
+    <s v="MVC folder hierarchy "/>
+    <x v="1"/>
+    <s v="Ersan Ünsal"/>
+    <x v="3"/>
+    <n v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="37.4"/>
+    <s v="Integrate our GoJS code to the new environment"/>
+    <s v="Code before refactoring works in new Pattern"/>
+    <x v="1"/>
+    <s v="Ersan Ünsal"/>
+    <x v="3"/>
+    <n v="3"/>
+    <x v="2"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="37.5"/>
+    <s v="Create models for our diagram"/>
+    <s v="Diagram generates objects "/>
+    <x v="2"/>
+    <s v="Karsten Rudolf"/>
+    <x v="3"/>
+    <n v="3"/>
+    <x v="2"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="37.6"/>
+    <s v="Create routes and controllers"/>
+    <s v="URL-handling Code"/>
+    <x v="4"/>
+    <s v="Edgar Meilinger"/>
+    <x v="3"/>
+    <n v="3"/>
+    <x v="2"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="37.7"/>
+    <s v="Testing communication with MongoDB"/>
+    <s v="Diagrams can be loaded and saved persistently in the Database"/>
+    <x v="6"/>
+    <m/>
+    <x v="4"/>
+    <m/>
+    <x v="3"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="37.7.1"/>
+    <s v="Implenting upload to database"/>
+    <s v="Upload to database available"/>
+    <x v="2"/>
+    <s v="Edgar Meilinger"/>
+    <x v="3"/>
+    <n v="6"/>
+    <x v="2"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="37.7.2."/>
+    <s v="Downloading from database"/>
+    <s v="Download to database available"/>
+    <x v="1"/>
+    <s v="Ersan Ünsal"/>
+    <x v="3"/>
+    <n v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <s v="Make Data Object reusable"/>
+    <s v="Reusing an existing Data Object, attached to different line "/>
+    <x v="6"/>
+    <m/>
+    <x v="4"/>
+    <m/>
+    <x v="3"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="38.1"/>
+    <s v="Research for making Data Object reusable"/>
+    <s v="Evaluate in which ways we can implent this task"/>
+    <x v="3"/>
+    <s v="Karsten Rudolf"/>
+    <x v="3"/>
+    <n v="3"/>
+    <x v="2"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="38.2"/>
+    <s v="Implenting a function to read and save all Data Objects and its values"/>
+    <s v="Making sure that we can work with the Data Objects and its values"/>
+    <x v="0"/>
+    <s v="Jan Leonardi"/>
+    <x v="3"/>
+    <n v="3"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="38.3"/>
+    <s v="Add this function into the listener and making sure it won't save duplicates"/>
+    <s v="Add this function into the listener and making sure it won't save duplicates"/>
+    <x v="0"/>
+    <s v="Jan Leonardi"/>
+    <x v="3"/>
+    <n v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="38.4"/>
+    <s v="Function to read and save Data Objects by name"/>
+    <s v="Function to read and save Data Objects by name"/>
+    <x v="3"/>
+    <s v="Karsten Rudolf"/>
+    <x v="3"/>
+    <n v="3"/>
+    <x v="2"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="38.5"/>
+    <s v="Implenting dropdown option for loading presets (Data Objects by name)"/>
+    <s v="Implenting dropdown option for loading presets (Data Objects by name)"/>
+    <x v="0"/>
+    <s v="Jan Leonardi"/>
+    <x v="3"/>
+    <n v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="38.6"/>
+    <s v="Implenting function into listener to fill Data Objects with the selected values from preset"/>
+    <s v="Implenting function into listener to fill Data Objects with the selected values from preset"/>
+    <x v="0"/>
+    <s v="Jan Leonardi"/>
+    <x v="3"/>
+    <n v="3"/>
+    <x v="2"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <s v="Data import: There is an Excel file with existing applications. _x000a_They need to be imported into the graphical editor, so that the additional applications are shown on the canvas."/>
+    <s v="Implementing an import option for excel files so you can see them on the canvas"/>
+    <x v="6"/>
+    <m/>
+    <x v="4"/>
+    <m/>
+    <x v="3"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="39.1"/>
+    <s v="Upload function"/>
+    <s v="Excel file can be uploaded temporaly into Server"/>
+    <x v="4"/>
+    <s v="Edgar Meilinger"/>
+    <x v="3"/>
+    <n v="4"/>
+    <x v="2"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="39.2"/>
+    <s v="Data cleaning"/>
+    <s v="All rows in the table which contains empty cells should be ignored and not converted to Application Object"/>
+    <x v="4"/>
+    <s v="Jan Leonardi"/>
+    <x v="3"/>
+    <n v="5"/>
+    <x v="2"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="39.3"/>
+    <s v="Add the imported apps to the diagram"/>
+    <s v="Imported Application should be added and shown in the diagram"/>
+    <x v="4"/>
+    <s v="Karsten Rudolf"/>
+    <x v="3"/>
+    <n v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3DBBB4A6-5CB7-4CEC-9E66-E98235078BFF}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:F12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="4"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="11">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="7"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Summe von Real Effort in h" fld="8" baseField="3" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1582,40 +2440,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" customWidth="1"/>
     <col min="2" max="2" width="121" customWidth="1"/>
-    <col min="3" max="3" width="91.140625" customWidth="1"/>
+    <col min="3" max="3" width="91.1796875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" customWidth="1"/>
+    <col min="8" max="8" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" customWidth="1"/>
+    <col min="11" max="11" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="28" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
@@ -1644,7 +2502,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -1673,7 +2531,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -1702,7 +2560,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>3</v>
       </c>
@@ -1731,7 +2589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>4</v>
       </c>
@@ -1760,7 +2618,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>5</v>
       </c>
@@ -1789,7 +2647,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>6</v>
       </c>
@@ -1818,7 +2676,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>7</v>
       </c>
@@ -1847,7 +2705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>8</v>
       </c>
@@ -1876,7 +2734,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>9</v>
       </c>
@@ -1905,7 +2763,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>10</v>
       </c>
@@ -1934,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>11</v>
       </c>
@@ -1963,7 +2821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
         <v>12</v>
       </c>
@@ -1992,7 +2850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="11">
         <v>13</v>
       </c>
@@ -2021,7 +2879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="11">
         <v>14</v>
       </c>
@@ -2050,7 +2908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="11">
         <v>15</v>
       </c>
@@ -2079,7 +2937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11">
         <v>16</v>
       </c>
@@ -2108,7 +2966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
         <v>17</v>
       </c>
@@ -2137,7 +2995,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="11">
         <v>18</v>
       </c>
@@ -2166,7 +3024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
         <v>19</v>
       </c>
@@ -2195,7 +3053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="11">
         <v>20</v>
       </c>
@@ -2224,7 +3082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="11">
         <v>21</v>
       </c>
@@ -2253,7 +3111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11">
         <v>22</v>
       </c>
@@ -2282,7 +3140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="11">
         <v>23</v>
       </c>
@@ -2311,7 +3169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="11">
         <v>24</v>
       </c>
@@ -2340,7 +3198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="11">
         <v>25</v>
       </c>
@@ -2369,7 +3227,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="11">
         <v>26</v>
       </c>
@@ -2398,7 +3256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
         <v>27</v>
       </c>
@@ -2427,7 +3285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="11">
         <v>28</v>
       </c>
@@ -2456,7 +3314,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="11">
         <v>29</v>
       </c>
@@ -2485,7 +3343,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="11">
         <v>30</v>
       </c>
@@ -2514,7 +3372,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="11">
         <v>31</v>
       </c>
@@ -2543,7 +3401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="11">
         <v>32</v>
       </c>
@@ -2572,7 +3430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>33</v>
       </c>
@@ -2601,7 +3459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>153</v>
       </c>
@@ -2629,9 +3487,9 @@
       <c r="I37" s="14">
         <v>2</v>
       </c>
-      <c r="L37" s="32"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L37" s="29"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>154</v>
       </c>
@@ -2659,9 +3517,9 @@
       <c r="I38" s="14">
         <v>1</v>
       </c>
-      <c r="L38" s="32"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L38" s="29"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>155</v>
       </c>
@@ -2689,9 +3547,9 @@
       <c r="I39" s="14">
         <v>2</v>
       </c>
-      <c r="L39" s="32"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L39" s="29"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="24">
         <v>35</v>
       </c>
@@ -2719,9 +3577,9 @@
       <c r="I40" s="16">
         <v>1</v>
       </c>
-      <c r="L40" s="32"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L40" s="29"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="24">
         <v>36</v>
       </c>
@@ -2737,9 +3595,9 @@
       <c r="G41" s="16"/>
       <c r="H41" s="15"/>
       <c r="I41" s="16"/>
-      <c r="L41" s="32"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L41" s="29"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
         <v>137</v>
       </c>
@@ -2768,7 +3626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="11" t="s">
         <v>138</v>
       </c>
@@ -2797,7 +3655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="24" t="s">
         <v>139</v>
       </c>
@@ -2826,7 +3684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
         <v>140</v>
       </c>
@@ -2855,7 +3713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
         <v>141</v>
       </c>
@@ -2884,7 +3742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
         <v>142</v>
       </c>
@@ -2913,7 +3771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>143</v>
       </c>
@@ -2930,11 +3788,11 @@
       <c r="H48" s="15"/>
       <c r="I48" s="16"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="28" t="s">
         <v>156</v>
       </c>
       <c r="C49" s="13" t="s">
@@ -2959,11 +3817,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="28" t="s">
         <v>157</v>
       </c>
       <c r="C50" s="13" t="s">
@@ -2988,7 +3846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="11">
         <v>38</v>
       </c>
@@ -3005,7 +3863,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="16"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
         <v>173</v>
       </c>
@@ -3034,7 +3892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
         <v>174</v>
       </c>
@@ -3063,7 +3921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="11" t="s">
         <v>181</v>
       </c>
@@ -3092,7 +3950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="11" t="s">
         <v>182</v>
       </c>
@@ -3121,7 +3979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="11" t="s">
         <v>183</v>
       </c>
@@ -3150,7 +4008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="11" t="s">
         <v>184</v>
       </c>
@@ -3179,7 +4037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="24">
         <v>39</v>
       </c>
@@ -3196,7 +4054,7 @@
       <c r="H58" s="13"/>
       <c r="I58" s="14"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="24" t="s">
         <v>162</v>
       </c>
@@ -3225,7 +4083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="24" t="s">
         <v>165</v>
       </c>
@@ -3254,7 +4112,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="24" t="s">
         <v>168</v>
       </c>
@@ -3317,14 +4175,14 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="74" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="5" width="17.85546875" customWidth="1"/>
+    <col min="4" max="5" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3341,7 +4199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3358,7 +4216,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3375,7 +4233,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3392,7 +4250,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3409,7 +4267,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3426,7 +4284,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3443,7 +4301,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3460,7 +4318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -3477,7 +4335,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -3494,7 +4352,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3503,7 +4361,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -3512,7 +4370,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -3521,7 +4379,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -3530,7 +4388,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -3539,7 +4397,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -3548,7 +4406,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -3557,7 +4415,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -3566,7 +4424,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -3575,7 +4433,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -3584,7 +4442,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -3593,7 +4451,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -3624,6 +4482,192 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F766830-04C4-499B-8B97-181CE7467FE7}">
+  <dimension ref="A3:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="22">
+        <v>6.5</v>
+      </c>
+      <c r="C5" s="22">
+        <v>12</v>
+      </c>
+      <c r="D5" s="22">
+        <v>14</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="22">
+        <v>4</v>
+      </c>
+      <c r="C6" s="22">
+        <v>7</v>
+      </c>
+      <c r="D6" s="22">
+        <v>11</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="22">
+        <v>6.5</v>
+      </c>
+      <c r="C7" s="22">
+        <v>11</v>
+      </c>
+      <c r="D7" s="22">
+        <v>12</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="22">
+        <v>5.5</v>
+      </c>
+      <c r="C9" s="22">
+        <v>12</v>
+      </c>
+      <c r="D9" s="22">
+        <v>11</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="22">
+        <v>11</v>
+      </c>
+      <c r="C10" s="22">
+        <v>7</v>
+      </c>
+      <c r="D10" s="22">
+        <v>11</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="22">
+        <v>34</v>
+      </c>
+      <c r="C12" s="22">
+        <v>49</v>
+      </c>
+      <c r="D12" s="22">
+        <v>59</v>
+      </c>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -3631,12 +4675,12 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -3647,7 +4691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3658,7 +4702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3669,7 +4713,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3680,7 +4724,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Report about the ignored apps is implemented
</commit_message>
<xml_diff>
--- a/Abgaben/Group_A_TaskRisk_log.xlsx
+++ b/Abgaben/Group_A_TaskRisk_log.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36792E10-DC89-4BAB-8CE2-723F536C2645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAF5558-4E95-4E25-AEC7-3B918389F63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="13230" windowWidth="29040" windowHeight="15840" tabRatio="412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -2533,25 +2533,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="121" customWidth="1"/>
-    <col min="3" max="3" width="97.7265625" customWidth="1"/>
+    <col min="3" max="3" width="97.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="19.453125" customWidth="1"/>
-    <col min="8" max="8" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" customWidth="1"/>
-    <col min="11" max="11" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>21</v>
       </c>
@@ -2566,7 +2566,7 @@
       <c r="H1" s="34"/>
       <c r="I1" s="35"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>3</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>4</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>5</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>6</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>7</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>8</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>9</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>10</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>11</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>12</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>13</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>14</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>15</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>16</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>17</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>18</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>19</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>20</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>21</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>22</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>23</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>24</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>25</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>26</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>27</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>28</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>29</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>30</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>31</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>32</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>33</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>172</v>
       </c>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="L37" s="29"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>173</v>
       </c>
@@ -3612,7 +3612,7 @@
       </c>
       <c r="L38" s="29"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>174</v>
       </c>
@@ -3642,7 +3642,7 @@
       </c>
       <c r="L39" s="29"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="24">
         <v>34</v>
       </c>
@@ -3672,7 +3672,7 @@
       </c>
       <c r="L40" s="29"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="24">
         <v>35</v>
       </c>
@@ -3690,7 +3690,7 @@
       <c r="I41" s="16"/>
       <c r="L41" s="29"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>181</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>182</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>183</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>184</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>185</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>186</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>187</v>
       </c>
@@ -3881,7 +3881,7 @@
       <c r="H48" s="15"/>
       <c r="I48" s="16"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>188</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>189</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>36</v>
       </c>
@@ -3956,7 +3956,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="16"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>175</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>176</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>177</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>178</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>179</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>180</v>
       </c>
@@ -4130,7 +4130,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="24">
         <v>37</v>
       </c>
@@ -4147,7 +4147,7 @@
       <c r="H58" s="13"/>
       <c r="I58" s="14"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
         <v>137</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
         <v>138</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
         <v>139</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="24">
         <v>38</v>
       </c>
@@ -4259,7 +4259,7 @@
       <c r="H62" s="15"/>
       <c r="I62" s="16"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="24">
         <v>39</v>
       </c>
@@ -4284,7 +4284,7 @@
       <c r="H63" s="15"/>
       <c r="I63" s="16"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="24">
         <v>40</v>
       </c>
@@ -4301,7 +4301,7 @@
       <c r="H64" s="15"/>
       <c r="I64" s="16"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
         <v>193</v>
       </c>
@@ -4326,7 +4326,7 @@
       <c r="H65" s="15"/>
       <c r="I65" s="16"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
         <v>196</v>
       </c>
@@ -4351,7 +4351,7 @@
       <c r="H66" s="15"/>
       <c r="I66" s="16"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="24" t="s">
         <v>198</v>
       </c>
@@ -4376,7 +4376,7 @@
       <c r="H67" s="15"/>
       <c r="I67" s="16"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="24">
         <v>41</v>
       </c>
@@ -4401,7 +4401,7 @@
       <c r="H68" s="15"/>
       <c r="I68" s="16"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="24">
         <v>42</v>
       </c>
@@ -4418,7 +4418,7 @@
       <c r="H69" s="15"/>
       <c r="I69" s="16"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="24" t="s">
         <v>204</v>
       </c>
@@ -4443,7 +4443,7 @@
       <c r="H70" s="15"/>
       <c r="I70" s="16"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
         <v>207</v>
       </c>
@@ -4468,7 +4468,7 @@
       <c r="H71" s="15"/>
       <c r="I71" s="16"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="24">
         <v>43</v>
       </c>
@@ -4493,7 +4493,7 @@
       <c r="H72" s="15"/>
       <c r="I72" s="16"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="24">
         <v>43</v>
       </c>
@@ -4518,7 +4518,7 @@
       <c r="H73" s="15"/>
       <c r="I73" s="16"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="24">
         <v>44</v>
       </c>
@@ -4543,7 +4543,7 @@
       <c r="H74" s="15"/>
       <c r="I74" s="16"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="24">
         <v>45</v>
       </c>
@@ -4558,7 +4558,7 @@
       <c r="H75" s="15"/>
       <c r="I75" s="16"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="24">
         <v>46</v>
       </c>
@@ -4575,7 +4575,7 @@
       <c r="H76" s="15"/>
       <c r="I76" s="16"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="24">
         <v>47</v>
       </c>
@@ -4590,7 +4590,7 @@
       <c r="H77" s="15"/>
       <c r="I77" s="16"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="24">
         <v>48</v>
       </c>
@@ -4639,14 +4639,14 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="74" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="5" width="17.81640625" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -4816,7 +4816,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -4825,7 +4825,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -4834,7 +4834,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -4843,7 +4843,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -4852,7 +4852,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -4861,7 +4861,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -4870,7 +4870,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -4879,7 +4879,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -4888,7 +4888,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -4897,7 +4897,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -4906,7 +4906,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -4915,7 +4915,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -4953,22 +4953,22 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>171</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>170</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>36</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>28</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>31</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>52</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>34</v>
       </c>
@@ -5082,7 +5082,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>24</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>168</v>
       </c>
@@ -5110,7 +5110,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>169</v>
       </c>
@@ -5141,12 +5141,12 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
update tasklist and retro 4
</commit_message>
<xml_diff>
--- a/Abgaben/Group_A_TaskRisk_log.xlsx
+++ b/Abgaben/Group_A_TaskRisk_log.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BC4F3A-E133-40E6-9D1E-B0A225CFEB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC131F4-8C82-4EA8-A258-A8F1F67FC6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-4290" windowWidth="29040" windowHeight="15840" tabRatio="412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="10" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="235">
   <si>
     <t>#</t>
   </si>
@@ -690,9 +690,6 @@
     <t>Research: Preset for excelsheets with same names</t>
   </si>
   <si>
-    <t>Multiple data objects for each data flow</t>
-  </si>
-  <si>
     <t>Automatic layout for nodes and bindings</t>
   </si>
   <si>
@@ -732,9 +729,6 @@
     <t>Make UI more userfriendly</t>
   </si>
   <si>
-    <t>Making DataObjects resuable</t>
-  </si>
-  <si>
     <t>38.5</t>
   </si>
   <si>
@@ -742,6 +736,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Refactor CSV export</t>
+  </si>
+  <si>
+    <t>Preset for excelsheets with same names</t>
+  </si>
+  <si>
+    <t>Making DataObjects resuable and multiable DataObjects for each link</t>
   </si>
 </sst>
 </file>
@@ -1417,19 +1417,19 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Autor" refreshedDate="44361.453187962965" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="58" xr:uid="{098F87A3-12ED-4463-A2D5-46F8DF234481}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Autor" refreshedDate="44372.934331365737" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="79" xr:uid="{098F87A3-12ED-4463-A2D5-46F8DF234481}">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabelle2"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="#" numFmtId="0">
-      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="39"/>
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="48"/>
     </cacheField>
     <cacheField name="Task" numFmtId="0">
       <sharedItems/>
     </cacheField>
     <cacheField name="Result" numFmtId="0">
-      <sharedItems/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Responsible" numFmtId="0">
       <sharedItems containsBlank="1" count="7">
@@ -1446,38 +1446,22 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Planned for Sprint #" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="3" count="5">
-        <n v="0"/>
-        <n v="1"/>
-        <n v="2"/>
-        <n v="3"/>
-        <m/>
-      </sharedItems>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="5"/>
     </cacheField>
     <cacheField name="Planned Effort in h" numFmtId="164">
       <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="6"/>
     </cacheField>
     <cacheField name="Realized in Sprint #" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="3" count="4">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="5">
         <n v="1"/>
         <n v="2"/>
         <n v="3"/>
         <m/>
+        <n v="4"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Real Effort in h" numFmtId="164">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="6" count="10">
-        <s v="5min"/>
-        <s v="2min"/>
-        <n v="1"/>
-        <n v="0.5"/>
-        <n v="6"/>
-        <n v="3"/>
-        <n v="2"/>
-        <n v="5"/>
-        <n v="4"/>
-        <m/>
-      </sharedItems>
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.5" maxValue="6"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -1489,17 +1473,17 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="58">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="79">
   <r>
     <n v="1"/>
     <s v="Creating a Discord Server for the Group"/>
     <s v="Voice communication &amp; Filesharing"/>
     <x v="0"/>
     <s v="Team"/>
+    <n v="0"/>
+    <s v="5min"/>
     <x v="0"/>
     <s v="5min"/>
-    <x v="0"/>
-    <x v="0"/>
   </r>
   <r>
     <n v="2"/>
@@ -1507,10 +1491,10 @@
     <s v="Text communication &amp; organising meetings"/>
     <x v="1"/>
     <s v="Team"/>
+    <n v="0"/>
+    <s v="2min"/>
     <x v="0"/>
     <s v="2min"/>
-    <x v="0"/>
-    <x v="1"/>
   </r>
   <r>
     <n v="3"/>
@@ -1518,10 +1502,10 @@
     <s v="Having phone numbers for the WhatsApp Group"/>
     <x v="2"/>
     <s v="Team"/>
-    <x v="0"/>
+    <n v="0"/>
     <n v="0.5"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="4"/>
@@ -1529,10 +1513,10 @@
     <s v="Get to know each other"/>
     <x v="3"/>
     <s v="Team"/>
+    <n v="0"/>
+    <n v="0.5"/>
     <x v="0"/>
     <n v="0.5"/>
-    <x v="0"/>
-    <x v="3"/>
   </r>
   <r>
     <n v="5"/>
@@ -1540,10 +1524,10 @@
     <s v="all have the same development enviroment"/>
     <x v="4"/>
     <s v="Team"/>
+    <n v="0"/>
+    <n v="0.5"/>
     <x v="0"/>
     <n v="0.5"/>
-    <x v="0"/>
-    <x v="3"/>
   </r>
   <r>
     <n v="6"/>
@@ -1551,10 +1535,10 @@
     <s v="sharing code &amp; version controlling"/>
     <x v="2"/>
     <s v="Team"/>
+    <n v="0"/>
+    <n v="0.5"/>
     <x v="0"/>
     <n v="0.5"/>
-    <x v="0"/>
-    <x v="3"/>
   </r>
   <r>
     <n v="7"/>
@@ -1562,10 +1546,10 @@
     <s v="sharing code &amp; version controlling"/>
     <x v="2"/>
     <s v="Team"/>
+    <n v="0"/>
+    <n v="1"/>
     <x v="0"/>
     <n v="1"/>
-    <x v="0"/>
-    <x v="2"/>
   </r>
   <r>
     <n v="8"/>
@@ -1573,10 +1557,10 @@
     <s v="understanding node.js, express, GoJS"/>
     <x v="0"/>
     <s v="Team"/>
+    <n v="0"/>
+    <n v="6"/>
     <x v="0"/>
     <n v="6"/>
-    <x v="0"/>
-    <x v="4"/>
   </r>
   <r>
     <n v="9"/>
@@ -1584,10 +1568,10 @@
     <s v="Getting an overview for what we have so far (will be extended in the future)"/>
     <x v="5"/>
     <s v="Team"/>
+    <n v="0"/>
+    <n v="0.5"/>
     <x v="0"/>
     <n v="0.5"/>
-    <x v="0"/>
-    <x v="3"/>
   </r>
   <r>
     <n v="10"/>
@@ -1595,10 +1579,10 @@
     <s v="Visual Background Canvas"/>
     <x v="3"/>
     <s v="Karsten Rudolf, Edgar Meilinger"/>
-    <x v="1"/>
+    <n v="1"/>
     <n v="2"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="11"/>
@@ -1606,10 +1590,10 @@
     <s v="Symbols can be created in the application"/>
     <x v="3"/>
     <s v="Karsten Rudolf, Edgar Meilinger"/>
-    <x v="1"/>
+    <n v="1"/>
     <n v="3"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="3"/>
   </r>
   <r>
     <n v="12"/>
@@ -1617,10 +1601,10 @@
     <s v="Elements can be moved freely in the application"/>
     <x v="3"/>
     <s v="Karsten Rudolf, Ersan Ünsal"/>
-    <x v="1"/>
+    <n v="1"/>
     <n v="1"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="13"/>
@@ -1628,10 +1612,10 @@
     <s v="Symbols can be dragged and dropped from the palette to the Main "/>
     <x v="2"/>
     <s v="Edgar Meilinger, Jan Leonardi"/>
-    <x v="1"/>
+    <n v="1"/>
     <n v="2"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="14"/>
@@ -1639,10 +1623,10 @@
     <s v="Application Design"/>
     <x v="0"/>
     <s v="Jan Leonardi, Ersan Ünsal"/>
-    <x v="1"/>
+    <n v="1"/>
     <n v="6"/>
     <x v="0"/>
-    <x v="7"/>
+    <n v="5"/>
   </r>
   <r>
     <n v="15"/>
@@ -1650,10 +1634,10 @@
     <s v="Basic documentation linked page for the customer"/>
     <x v="2"/>
     <s v="Edgar Meilinger"/>
-    <x v="1"/>
+    <n v="1"/>
     <n v="2"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="16"/>
@@ -1661,10 +1645,10 @@
     <s v="The properties can be shown using a properties window"/>
     <x v="1"/>
     <s v="Jan Leonardi, Gökhan Ünsal"/>
-    <x v="1"/>
+    <n v="1"/>
     <n v="4"/>
     <x v="0"/>
-    <x v="8"/>
+    <n v="4"/>
   </r>
   <r>
     <n v="17"/>
@@ -1672,10 +1656,10 @@
     <s v="Applications can be connected with directed associations (arrowheads) representing dataflows. "/>
     <x v="4"/>
     <s v="Gökhan Ünsal, Ersan Ünsal"/>
-    <x v="1"/>
+    <n v="1"/>
     <n v="6"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="6"/>
   </r>
   <r>
     <n v="18"/>
@@ -1683,10 +1667,10 @@
     <s v="With following properties: Name, description &amp; personal data ? Dataflow refers to Data Object"/>
     <x v="4"/>
     <s v="Edgar Meilinger"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="4"/>
     <x v="1"/>
-    <x v="8"/>
+    <n v="4"/>
   </r>
   <r>
     <n v="19"/>
@@ -1694,10 +1678,10 @@
     <s v="Label is like a node; display name, description &amp; personal data"/>
     <x v="4"/>
     <s v="Gökhan Ünsal"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="6"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="6"/>
   </r>
   <r>
     <n v="20"/>
@@ -1705,10 +1689,10 @@
     <s v="Application will appear as default by the name &quot;Application&quot; and not as &quot;Program&quot;"/>
     <x v="0"/>
     <s v="Edgar Meilinger"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="1"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="1"/>
   </r>
   <r>
     <n v="21"/>
@@ -1716,10 +1700,10 @@
     <s v="Properties dialog will only be visible when you click on the Application"/>
     <x v="3"/>
     <s v="Karsten Rudolf"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="2"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="22"/>
@@ -1727,10 +1711,10 @@
     <s v="Property window for links will only show &quot;name&quot; &amp; &quot;color&quot;"/>
     <x v="4"/>
     <s v="Jan Leonardi"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="2"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="2"/>
   </r>
   <r>
     <n v="23"/>
@@ -1738,10 +1722,10 @@
     <s v="Gathering information about how GoJS saves data to use it for the traffic light"/>
     <x v="0"/>
     <s v="Ersan Ünsal"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="3"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="3"/>
   </r>
   <r>
     <n v="24"/>
@@ -1749,10 +1733,10 @@
     <s v="Implementing traffic light system for Applications the have a visual overview for the status"/>
     <x v="2"/>
     <s v="Karsten Rudolf"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="5"/>
     <x v="1"/>
-    <x v="7"/>
+    <n v="5"/>
   </r>
   <r>
     <n v="25"/>
@@ -1760,10 +1744,10 @@
     <s v="Changing free text value for COTS into a dropdown menu with 3 values(cots, propietary, undefined)"/>
     <x v="0"/>
     <s v="Ersan Ünsal"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="3"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="3"/>
   </r>
   <r>
     <n v="26"/>
@@ -1771,10 +1755,10 @@
     <s v="Change input filed to textarea"/>
     <x v="1"/>
     <s v="Jan Leonardi"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="3"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="3"/>
   </r>
   <r>
     <n v="27"/>
@@ -1782,10 +1766,10 @@
     <s v="Changing the visual desgin of the symbol for the applications"/>
     <x v="1"/>
     <s v="Ersan Ünsal"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="4"/>
     <x v="1"/>
-    <x v="8"/>
+    <n v="4"/>
   </r>
   <r>
     <n v="28"/>
@@ -1793,10 +1777,10 @@
     <s v="Being able to solve the export tasks"/>
     <x v="3"/>
     <s v="Amine Amzil"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="6"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="6"/>
   </r>
   <r>
     <n v="29"/>
@@ -1804,10 +1788,10 @@
     <s v="Diagramm data can be shown as JSON"/>
     <x v="2"/>
     <s v="Jan Leonardi"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="3"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="3"/>
   </r>
   <r>
     <n v="30"/>
@@ -1815,10 +1799,10 @@
     <s v="Implenting an export option to save &amp; report all data objects in the application landscape as an .csv file"/>
     <x v="3"/>
     <s v="Amine Amzil"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="4"/>
     <x v="1"/>
-    <x v="8"/>
+    <n v="4"/>
   </r>
   <r>
     <n v="31"/>
@@ -1826,10 +1810,10 @@
     <s v="Communication between app and database"/>
     <x v="2"/>
     <s v="Karsten Rudolf"/>
-    <x v="2"/>
+    <n v="2"/>
     <n v="3"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="3"/>
   </r>
   <r>
     <n v="32"/>
@@ -1837,10 +1821,10 @@
     <s v="Implementing more visible lines in the fields of description"/>
     <x v="1"/>
     <s v="Jan Leonardi"/>
+    <n v="2"/>
+    <n v="3"/>
     <x v="2"/>
     <n v="3"/>
-    <x v="2"/>
-    <x v="5"/>
   </r>
   <r>
     <n v="33"/>
@@ -1848,292 +1832,523 @@
     <s v="Implenting an export option to save &amp; report all data in the application related with personal data"/>
     <x v="0"/>
     <s v="Jan Leonardi"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="3"/>
     <x v="2"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <s v="34.1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="33.1"/>
     <s v="Debugging"/>
     <s v="Fixing bugs"/>
     <x v="3"/>
     <s v="Karsten Rudolf"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="2"/>
     <x v="2"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <s v="34.2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="33.2"/>
     <s v="Download component"/>
     <s v="Download component"/>
     <x v="3"/>
     <s v="Karsten Rudolf"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="1"/>
     <x v="2"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="34.3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="33.3"/>
     <s v="Time component"/>
     <s v="Time component"/>
     <x v="3"/>
     <s v="Karsten Rudolf"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="2"/>
     <x v="2"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <n v="35"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="34"/>
     <s v="Rename the Status to COTS Label"/>
     <s v="Changing visual text from status to COTS"/>
     <x v="2"/>
     <s v="Edgar Meilinger"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="1"/>
     <x v="2"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="36"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="35"/>
     <s v="Refactoring the Code"/>
     <s v="Application landscape has to be stored persistently e.g. as Database"/>
     <x v="6"/>
     <m/>
-    <x v="4"/>
+    <m/>
     <m/>
     <x v="3"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <s v="37.1"/>
+    <m/>
+  </r>
+  <r>
+    <s v="35.1"/>
     <s v="Research for MVC-Pattern in NodeJs"/>
     <s v="Using a Module for MVC Pattern"/>
     <x v="2"/>
     <s v="Amine Amzil"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="1"/>
     <x v="2"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="37.2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="35.2"/>
     <s v="Creating a plan for refactoring"/>
     <s v="Organising for the tasks to refactor the code"/>
     <x v="2"/>
     <s v="Amine Amzil"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="2"/>
     <x v="2"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <s v="37.3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="35.3"/>
     <s v="Generating a MVC Skeleton"/>
     <s v="MVC folder hierarchy "/>
     <x v="1"/>
     <s v="Ersan Ünsal"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="2"/>
     <x v="2"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <s v="37.4"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="35.4"/>
     <s v="Integrate our GoJS code to the new environment"/>
     <s v="Code before refactoring works in new Pattern"/>
     <x v="1"/>
     <s v="Ersan Ünsal"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="3"/>
     <x v="2"/>
-    <x v="8"/>
-  </r>
-  <r>
-    <s v="37.5"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="35.5"/>
     <s v="Create models for our diagram"/>
     <s v="Diagram generates objects "/>
     <x v="2"/>
     <s v="Karsten Rudolf"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="3"/>
     <x v="2"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <s v="37.6"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="35.6"/>
     <s v="Create routes and controllers"/>
     <s v="URL-handling Code"/>
     <x v="4"/>
     <s v="Edgar Meilinger"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="3"/>
     <x v="2"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <s v="37.7"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="35.7"/>
     <s v="Testing communication with MongoDB"/>
     <s v="Diagrams can be loaded and saved persistently in the Database"/>
     <x v="6"/>
     <m/>
-    <x v="4"/>
+    <m/>
     <m/>
     <x v="3"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <s v="37.7.1"/>
+    <m/>
+  </r>
+  <r>
+    <s v="35.7.1"/>
     <s v="Implenting upload to database"/>
     <s v="Upload to database available"/>
     <x v="2"/>
     <s v="Edgar Meilinger"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="6"/>
     <x v="2"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <s v="37.7.2."/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="35.7.2."/>
     <s v="Downloading from database"/>
     <s v="Download to database available"/>
     <x v="1"/>
     <s v="Ersan Ünsal"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="2"/>
     <x v="2"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <n v="38"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="36"/>
     <s v="Make Data Object reusable"/>
     <s v="Reusing an existing Data Object, attached to different line "/>
     <x v="6"/>
     <m/>
-    <x v="4"/>
+    <m/>
     <m/>
     <x v="3"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <s v="38.1"/>
+    <m/>
+  </r>
+  <r>
+    <s v="36.1"/>
     <s v="Research for making Data Object reusable"/>
     <s v="Evaluate in which ways we can implent this task"/>
     <x v="3"/>
     <s v="Karsten Rudolf"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="3"/>
     <x v="2"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <s v="38.2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="36.2"/>
     <s v="Implenting a function to read and save all Data Objects and its values"/>
     <s v="Making sure that we can work with the Data Objects and its values"/>
     <x v="0"/>
     <s v="Jan Leonardi"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="3"/>
     <x v="2"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <s v="38.3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="36.3"/>
     <s v="Add this function into the listener and making sure it won't save duplicates"/>
     <s v="Add this function into the listener and making sure it won't save duplicates"/>
     <x v="0"/>
     <s v="Jan Leonardi"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="2"/>
     <x v="2"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <s v="38.4"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="36.4"/>
     <s v="Function to read and save Data Objects by name"/>
     <s v="Function to read and save Data Objects by name"/>
     <x v="3"/>
     <s v="Karsten Rudolf"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="3"/>
     <x v="2"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <s v="38.5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="36.5"/>
     <s v="Implenting dropdown option for loading presets (Data Objects by name)"/>
     <s v="Implenting dropdown option for loading presets (Data Objects by name)"/>
     <x v="0"/>
     <s v="Jan Leonardi"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="2"/>
     <x v="2"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <s v="38.6"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="36.6"/>
     <s v="Implenting function into listener to fill Data Objects with the selected values from preset"/>
     <s v="Implenting function into listener to fill Data Objects with the selected values from preset"/>
     <x v="0"/>
     <s v="Jan Leonardi"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="3"/>
     <x v="2"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <n v="39"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="37"/>
     <s v="Data import: There is an Excel file with existing applications. _x000a_They need to be imported into the graphical editor, so that the additional applications are shown on the canvas."/>
     <s v="Implementing an import option for excel files so you can see them on the canvas"/>
     <x v="6"/>
     <m/>
-    <x v="4"/>
+    <m/>
     <m/>
     <x v="3"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <s v="39.1"/>
+    <m/>
+  </r>
+  <r>
+    <s v="37.1"/>
     <s v="Upload function"/>
     <s v="Excel file can be uploaded temporaly into Server"/>
     <x v="4"/>
     <s v="Edgar Meilinger"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="4"/>
     <x v="2"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <s v="39.2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="37.2"/>
     <s v="Data cleaning"/>
     <s v="All rows in the table which contains empty cells should be ignored and not converted to Application Object"/>
     <x v="4"/>
     <s v="Jan Leonardi"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="5"/>
     <x v="2"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <s v="39.3"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <s v="37.3"/>
     <s v="Add the imported apps to the diagram"/>
     <s v="Imported Application should be added and shown in the diagram"/>
     <x v="4"/>
     <s v="Karsten Rudolf"/>
-    <x v="3"/>
+    <n v="3"/>
     <n v="2"/>
     <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <s v="Making DataObjects resuable and multiable DataObjects for each link"/>
+    <m/>
     <x v="6"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <m/>
+  </r>
+  <r>
+    <s v="38.1"/>
+    <s v="Refactoring for multiple DataObjects"/>
+    <s v="Refactoring to be able to implement multiple DataObjects"/>
+    <x v="3"/>
+    <s v="Ersan Ünsal"/>
+    <n v="4"/>
+    <n v="4"/>
+    <x v="3"/>
+    <m/>
+  </r>
+  <r>
+    <s v="38.2"/>
+    <s v="Load and edit Data Objects"/>
+    <s v="Visualized as table so you can choose and edit from this table"/>
+    <x v="3"/>
+    <s v="Edgar Meilinger"/>
+    <n v="4"/>
+    <n v="4"/>
+    <x v="3"/>
+    <m/>
+  </r>
+  <r>
+    <s v="38.3"/>
+    <s v="Delete DataObjects"/>
+    <s v="Being able to choose DataObjects from table and delete it"/>
+    <x v="3"/>
+    <s v="Karsten Rudolf"/>
+    <n v="5"/>
+    <n v="2"/>
+    <x v="3"/>
+    <m/>
+  </r>
+  <r>
+    <s v="38.4"/>
+    <s v="Editing design for table etc."/>
+    <s v="Make UI more userfriendly"/>
+    <x v="0"/>
+    <s v="Jan Leonardi"/>
+    <n v="5"/>
+    <n v="4"/>
+    <x v="3"/>
+    <m/>
+  </r>
+  <r>
+    <s v="38.5"/>
+    <s v=" Refactor CSV export"/>
+    <s v="Export to CSV has to be refactored"/>
+    <x v="3"/>
+    <s v="Karsten Rudolf"/>
+    <n v="5"/>
+    <n v="5"/>
+    <x v="3"/>
+    <m/>
+  </r>
+  <r>
+    <n v="39"/>
+    <s v="Rename Preset into customer terms (Reusable Data Objects)"/>
+    <s v="Rename Preset into costumer terms (Reusable Data Objects)"/>
+    <x v="1"/>
+    <s v="Amine Amzil"/>
+    <n v="4"/>
+    <n v="1"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="40"/>
+    <s v="Customising User Interface"/>
+    <m/>
+    <x v="6"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <m/>
+  </r>
+  <r>
+    <s v="40.1"/>
+    <s v="Rearranging Import- / Export- / Save- and Loadbuttons"/>
+    <s v="Making the UI more User friendly"/>
+    <x v="0"/>
+    <s v="Jan Leonardi"/>
+    <n v="4"/>
+    <n v="4"/>
+    <x v="4"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="40.2"/>
+    <s v="Creating our own window and replacing inspector for Data Objects"/>
+    <s v="Making the UI more User friendly"/>
+    <x v="0"/>
+    <s v="Jan Leonardi"/>
+    <n v="4"/>
+    <n v="3"/>
+    <x v="3"/>
+    <m/>
+  </r>
+  <r>
+    <s v="40.3"/>
+    <s v="Greeting Screen"/>
+    <s v="Options to select Diagrams from the database (as a list), creating a new diagram or import diagram from Excel/csv"/>
+    <x v="2"/>
+    <s v="Amine Amzil"/>
+    <n v="4"/>
+    <n v="3"/>
+    <x v="4"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <n v="41"/>
+    <s v="Option for saving and loading multiple diagrams from the Database"/>
+    <s v="Diagrams have their own unique keys, so they can be loaded and saved from/into the database"/>
+    <x v="2"/>
+    <s v="Edgar Meilinger"/>
+    <n v="4"/>
+    <n v="5"/>
+    <x v="4"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <n v="42"/>
+    <s v="Customising Excel import window"/>
+    <m/>
+    <x v="6"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <m/>
+  </r>
+  <r>
+    <s v="42.1"/>
+    <s v="User doesn't need to fill out each tabs -&gt; dropdown option with preloaded values"/>
+    <s v="Mitigation of User errors and more user friendly"/>
+    <x v="4"/>
+    <s v="Edgar Meilinger"/>
+    <n v="4"/>
+    <n v="4"/>
+    <x v="3"/>
+    <m/>
+  </r>
+  <r>
+    <s v="42.2"/>
+    <s v="Error report list for the failed to import data"/>
+    <s v="Getting information of the Data that didn't get imported"/>
+    <x v="4"/>
+    <s v="Edgar Meilinger"/>
+    <n v="4"/>
+    <n v="4"/>
+    <x v="4"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <s v="Research: Multiple data objects for each data flow ( How many are possible ? )"/>
+    <s v="Checking if its possible"/>
+    <x v="1"/>
+    <s v="Jan Leonardi"/>
+    <n v="4"/>
+    <n v="4"/>
+    <x v="3"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <s v="Research: Automated mapping/layout for the diagram"/>
+    <s v="Checking if its possible"/>
+    <x v="1"/>
+    <s v="Karsten Rudolf"/>
+    <n v="4"/>
+    <n v="4"/>
+    <x v="3"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <n v="44"/>
+    <s v="Refactoring html into pug for views"/>
+    <s v="Frontend is now fully unified over controllers"/>
+    <x v="1"/>
+    <s v="Ersan Ünsal"/>
+    <n v="4"/>
+    <n v="3"/>
+    <x v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="45"/>
+    <s v="Database Credentials are accessable in the application"/>
+    <m/>
+    <x v="6"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+    <m/>
+  </r>
+  <r>
+    <n v="46"/>
+    <s v="Research: Preset for excelsheets with same names"/>
+    <s v="Preset for excelsheets with same names"/>
+    <x v="4"/>
+    <s v="Jan Leonardi"/>
+    <n v="4"/>
+    <n v="3"/>
+    <x v="4"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="48"/>
+    <s v="Automatic layout for nodes and bindings"/>
+    <s v="Making the UI more User friendly"/>
+    <x v="1"/>
+    <s v="Amine Amzil"/>
+    <n v="4"/>
+    <n v="5"/>
+    <x v="3"/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3DBBB4A6-5CB7-4CEC-9E66-E98235078BFF}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:F12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3DBBB4A6-5CB7-4CEC-9E66-E98235078BFF}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -2151,41 +2366,19 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField showAll="0">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
       <items count="6">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item x="3"/>
         <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
         <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" showAll="0">
-      <items count="11">
-        <item x="3"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="3"/>
@@ -2219,7 +2412,7 @@
   <colFields count="1">
     <field x="7"/>
   </colFields>
-  <colItems count="5">
+  <colItems count="6">
     <i>
       <x/>
     </i>
@@ -2231,6 +2424,9 @@
     </i>
     <i>
       <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -2252,8 +2448,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="A3:I83" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A3:I83" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="A3:I82" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+  <autoFilter ref="A3:I82" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task" dataDxfId="19"/>
@@ -2576,27 +2772,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L83"/>
+  <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="121" customWidth="1"/>
-    <col min="3" max="3" width="97.7265625" customWidth="1"/>
+    <col min="3" max="3" width="97.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="19.453125" customWidth="1"/>
-    <col min="8" max="8" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" customWidth="1"/>
-    <col min="11" max="11" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>21</v>
       </c>
@@ -2611,7 +2807,7 @@
       <c r="H1" s="34"/>
       <c r="I1" s="35"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
@@ -2640,7 +2836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -2669,7 +2865,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -2698,7 +2894,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>3</v>
       </c>
@@ -2727,7 +2923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>4</v>
       </c>
@@ -2756,7 +2952,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>5</v>
       </c>
@@ -2785,7 +2981,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>6</v>
       </c>
@@ -2814,7 +3010,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>7</v>
       </c>
@@ -2843,7 +3039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>8</v>
       </c>
@@ -2872,7 +3068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>9</v>
       </c>
@@ -2901,7 +3097,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>10</v>
       </c>
@@ -2930,7 +3126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>11</v>
       </c>
@@ -2959,7 +3155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>12</v>
       </c>
@@ -2988,7 +3184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>13</v>
       </c>
@@ -3017,7 +3213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>14</v>
       </c>
@@ -3046,7 +3242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>15</v>
       </c>
@@ -3075,7 +3271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>16</v>
       </c>
@@ -3104,7 +3300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>17</v>
       </c>
@@ -3133,7 +3329,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>18</v>
       </c>
@@ -3162,7 +3358,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>19</v>
       </c>
@@ -3191,7 +3387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>20</v>
       </c>
@@ -3220,7 +3416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>21</v>
       </c>
@@ -3249,7 +3445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>22</v>
       </c>
@@ -3278,7 +3474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>23</v>
       </c>
@@ -3307,7 +3503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>24</v>
       </c>
@@ -3336,7 +3532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>25</v>
       </c>
@@ -3365,7 +3561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>26</v>
       </c>
@@ -3394,7 +3590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>27</v>
       </c>
@@ -3423,7 +3619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>28</v>
       </c>
@@ -3452,7 +3648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>29</v>
       </c>
@@ -3481,7 +3677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>30</v>
       </c>
@@ -3510,7 +3706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>31</v>
       </c>
@@ -3539,7 +3735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>32</v>
       </c>
@@ -3568,7 +3764,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>33</v>
       </c>
@@ -3597,7 +3793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>172</v>
       </c>
@@ -3627,7 +3823,7 @@
       </c>
       <c r="L37" s="29"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>173</v>
       </c>
@@ -3657,7 +3853,7 @@
       </c>
       <c r="L38" s="29"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>174</v>
       </c>
@@ -3687,7 +3883,7 @@
       </c>
       <c r="L39" s="29"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="24">
         <v>34</v>
       </c>
@@ -3717,7 +3913,7 @@
       </c>
       <c r="L40" s="29"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="24">
         <v>35</v>
       </c>
@@ -3735,7 +3931,7 @@
       <c r="I41" s="16"/>
       <c r="L41" s="29"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>181</v>
       </c>
@@ -3764,7 +3960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>182</v>
       </c>
@@ -3793,7 +3989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>183</v>
       </c>
@@ -3822,7 +4018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>184</v>
       </c>
@@ -3851,7 +4047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>185</v>
       </c>
@@ -3880,7 +4076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>186</v>
       </c>
@@ -3909,7 +4105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>187</v>
       </c>
@@ -3926,7 +4122,7 @@
       <c r="H48" s="15"/>
       <c r="I48" s="16"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>188</v>
       </c>
@@ -3955,7 +4151,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>189</v>
       </c>
@@ -3984,7 +4180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>36</v>
       </c>
@@ -4001,7 +4197,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="16"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>175</v>
       </c>
@@ -4030,7 +4226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>176</v>
       </c>
@@ -4059,7 +4255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>177</v>
       </c>
@@ -4088,7 +4284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>178</v>
       </c>
@@ -4117,7 +4313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>179</v>
       </c>
@@ -4146,7 +4342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>180</v>
       </c>
@@ -4175,7 +4371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="24">
         <v>37</v>
       </c>
@@ -4192,7 +4388,7 @@
       <c r="H58" s="13"/>
       <c r="I58" s="14"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
         <v>137</v>
       </c>
@@ -4221,7 +4417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
         <v>138</v>
       </c>
@@ -4250,7 +4446,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
         <v>139</v>
       </c>
@@ -4279,12 +4475,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="24">
         <v>38</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C62" s="23"/>
       <c r="D62" s="15"/>
@@ -4294,15 +4490,15 @@
       <c r="H62" s="15"/>
       <c r="I62" s="16"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B63" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="B63" s="12" t="s">
+      <c r="C63" s="12" t="s">
         <v>220</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>221</v>
       </c>
       <c r="D63" s="13" t="s">
         <v>34</v>
@@ -4319,15 +4515,15 @@
       <c r="H63" s="13"/>
       <c r="I63" s="14"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B64" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="B64" s="12" t="s">
-        <v>223</v>
-      </c>
       <c r="C64" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D64" s="13" t="s">
         <v>34</v>
@@ -4344,15 +4540,15 @@
       <c r="H64" s="13"/>
       <c r="I64" s="14"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="B65" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="B65" s="12" t="s">
-        <v>225</v>
-      </c>
       <c r="C65" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D65" s="13" t="s">
         <v>34</v>
@@ -4369,15 +4565,15 @@
       <c r="H65" s="13"/>
       <c r="I65" s="14"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="B66" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="B66" s="12" t="s">
+      <c r="C66" s="12" t="s">
         <v>229</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>230</v>
       </c>
       <c r="D66" s="13" t="s">
         <v>24</v>
@@ -4394,15 +4590,15 @@
       <c r="H66" s="13"/>
       <c r="I66" s="14"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B67" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="B67" s="12" t="s">
-        <v>234</v>
-      </c>
       <c r="C67" s="12" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D67" s="13" t="s">
         <v>34</v>
@@ -4419,7 +4615,7 @@
       <c r="H67" s="13"/>
       <c r="I67" s="14"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="24">
         <v>39</v>
       </c>
@@ -4448,7 +4644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="24">
         <v>40</v>
       </c>
@@ -4463,7 +4659,7 @@
       <c r="H69" s="15"/>
       <c r="I69" s="16"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="24" t="s">
         <v>192</v>
       </c>
@@ -4492,7 +4688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
         <v>195</v>
       </c>
@@ -4517,7 +4713,7 @@
       <c r="H71" s="15"/>
       <c r="I71" s="16"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="24" t="s">
         <v>197</v>
       </c>
@@ -4546,7 +4742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="24">
         <v>41</v>
       </c>
@@ -4575,7 +4771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="24">
         <v>42</v>
       </c>
@@ -4585,14 +4781,12 @@
       <c r="C74" s="15"/>
       <c r="D74" s="15"/>
       <c r="E74" s="15"/>
-      <c r="F74" s="25">
-        <v>4</v>
-      </c>
+      <c r="F74" s="25"/>
       <c r="G74" s="16"/>
       <c r="H74" s="15"/>
       <c r="I74" s="16"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
         <v>203</v>
       </c>
@@ -4617,7 +4811,7 @@
       <c r="H75" s="15"/>
       <c r="I75" s="16"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
         <v>206</v>
       </c>
@@ -4639,10 +4833,14 @@
       <c r="G76" s="16">
         <v>4</v>
       </c>
-      <c r="H76" s="15"/>
-      <c r="I76" s="16"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H76" s="15">
+        <v>4</v>
+      </c>
+      <c r="I76" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="24">
         <v>43</v>
       </c>
@@ -4669,7 +4867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="24">
         <v>43</v>
       </c>
@@ -4696,7 +4894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="24">
         <v>44</v>
       </c>
@@ -4723,7 +4921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="24">
         <v>45</v>
       </c>
@@ -4738,14 +4936,16 @@
       <c r="H80" s="15"/>
       <c r="I80" s="16"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="24">
         <v>46</v>
       </c>
       <c r="B81" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="C81" s="15"/>
+      <c r="C81" s="15" t="s">
+        <v>233</v>
+      </c>
       <c r="D81" s="15" t="s">
         <v>36</v>
       </c>
@@ -4756,40 +4956,39 @@
         <v>4</v>
       </c>
       <c r="G81" s="16">
+        <v>3</v>
+      </c>
+      <c r="H81" s="15">
         <v>4</v>
       </c>
-      <c r="H81" s="15"/>
-      <c r="I81" s="16"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I81" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="24">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B82" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="C82" s="15"/>
-      <c r="D82" s="15"/>
-      <c r="E82" s="15"/>
-      <c r="F82" s="25"/>
-      <c r="G82" s="16"/>
+      <c r="C82" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E82" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F82" s="25">
+        <v>4</v>
+      </c>
+      <c r="G82" s="16">
+        <v>5</v>
+      </c>
       <c r="H82" s="15"/>
       <c r="I82" s="16"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A83" s="24">
-        <v>48</v>
-      </c>
-      <c r="B83" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="C83" s="15"/>
-      <c r="D83" s="15"/>
-      <c r="E83" s="15"/>
-      <c r="F83" s="25"/>
-      <c r="G83" s="16"/>
-      <c r="H83" s="15"/>
-      <c r="I83" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4825,14 +5024,14 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="74" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="5" width="17.81640625" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4849,7 +5048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -4866,7 +5065,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -4883,7 +5082,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -4900,7 +5099,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -4917,7 +5116,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -4934,7 +5133,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -4951,7 +5150,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -4968,7 +5167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -4985,7 +5184,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -5002,7 +5201,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -5011,7 +5210,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -5020,7 +5219,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -5029,7 +5228,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -5038,7 +5237,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -5047,7 +5246,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -5056,7 +5255,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -5065,7 +5264,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -5074,7 +5273,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -5083,7 +5282,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -5092,7 +5291,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -5101,7 +5300,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -5133,28 +5332,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F766830-04C4-499B-8B97-181CE7467FE7}">
-  <dimension ref="A3:F12"/>
+  <dimension ref="A3:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I8" sqref="I8:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>171</v>
       </c>
@@ -5162,7 +5371,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>170</v>
       </c>
@@ -5175,14 +5384,17 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
         <v>168</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>36</v>
       </c>
@@ -5195,12 +5407,15 @@
       <c r="D5" s="22">
         <v>14</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22">
-        <v>32.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E5" s="22">
+        <v>6</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>28</v>
       </c>
@@ -5213,12 +5428,17 @@
       <c r="D6" s="22">
         <v>11</v>
       </c>
-      <c r="E6" s="22"/>
+      <c r="E6" s="22">
+        <v>1</v>
+      </c>
       <c r="F6" s="22">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="G6" s="22">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>31</v>
       </c>
@@ -5231,12 +5451,15 @@
       <c r="D7" s="22">
         <v>12</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22">
-        <v>29.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E7" s="22">
+        <v>8</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>52</v>
       </c>
@@ -5246,11 +5469,12 @@
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
-      <c r="F8" s="22">
+      <c r="F8" s="22"/>
+      <c r="G8" s="22">
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>34</v>
       </c>
@@ -5264,11 +5488,12 @@
         <v>11</v>
       </c>
       <c r="E9" s="22"/>
-      <c r="F9" s="22">
+      <c r="F9" s="22"/>
+      <c r="G9" s="22">
         <v>28.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>24</v>
       </c>
@@ -5281,12 +5506,15 @@
       <c r="D10" s="22">
         <v>11</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E10" s="22">
+        <v>5</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>168</v>
       </c>
@@ -5295,8 +5523,9 @@
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="22"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>169</v>
       </c>
@@ -5309,9 +5538,14 @@
       <c r="D12" s="22">
         <v>59</v>
       </c>
-      <c r="E12" s="22"/>
+      <c r="E12" s="22">
+        <v>20</v>
+      </c>
       <c r="F12" s="22">
-        <v>142</v>
+        <v>11</v>
+      </c>
+      <c r="G12" s="22">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -5327,12 +5561,12 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -5343,7 +5577,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5354,7 +5588,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5365,7 +5599,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5376,7 +5610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>